<commit_message>
[SIT] Update import user
</commit_message>
<xml_diff>
--- a/apps/core/fimport/static/fimport/template/af9c6fd3-1815-4d5a-aa24-fca9d095cb7a.xlsx
+++ b/apps/core/fimport/static/fimport/template/af9c6fd3-1815-4d5a-aa24-fca9d095cb7a.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nguyen Tong Trieu\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Coding\MIS\misui\apps\core\fimport\static\fimport\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F663B47-5D8F-42C6-AD36-89E58528A7B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06CF0CE6-11C3-42B0-8EFC-7D5764F53EC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ABCF866D-F0C2-489F-81F3-6B45D3E3629E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ABCF866D-F0C2-489F-81F3-6B45D3E3629E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,16 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t xml:space="preserve">Tên đăng nhập </t>
-  </si>
-  <si>
-    <t>Họ</t>
-  </si>
-  <si>
-    <t>Tên</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>E-Mail</t>
   </si>
@@ -43,14 +34,34 @@
   </si>
   <si>
     <t>STT</t>
+  </si>
+  <si>
+    <t>Tên đăng nhập (*)</t>
+  </si>
+  <si>
+    <t>Họ (*)</t>
+  </si>
+  <si>
+    <t>Tên (*)</t>
+  </si>
+  <si>
+    <t>Mật khẩu (*)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -66,7 +77,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -74,12 +85,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBA1278D-5766-4C30-B51D-59CB3DF80128}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -405,32 +432,35 @@
     <col min="1" max="1" width="5.88671875" customWidth="1"/>
     <col min="2" max="2" width="18.33203125" customWidth="1"/>
     <col min="3" max="3" width="19.21875" customWidth="1"/>
-    <col min="4" max="4" width="15.88671875" customWidth="1"/>
-    <col min="5" max="5" width="36.6640625" customWidth="1"/>
-    <col min="6" max="6" width="22" customWidth="1"/>
+    <col min="4" max="5" width="15.88671875" customWidth="1"/>
+    <col min="6" max="6" width="36.6640625" customWidth="1"/>
+    <col min="7" max="7" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>IF(ISBLANK(B2), "", ROW(A2) -1)</f>
         <v/>

</xml_diff>